<commit_message>
Fixed priority calc bug, made changes for oculus tests, pretty gizmos in editor
</commit_message>
<xml_diff>
--- a/test/HDR-VDP/hdrvdp-3.0.7/test_move/Test-1-SP/10/vdp-hdr-detection.xlsx
+++ b/test/HDR-VDP/hdrvdp-3.0.7/test_move/Test-1-SP/10/vdp-hdr-detection.xlsx
@@ -64,297 +64,297 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0">
-        <v>0.99873788144865738</v>
+        <v>0.30261196328375123</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>0.99929504107090794</v>
+        <v>0.22278057385692498</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>0.89775061621788821</v>
+        <v>0.68958690916092702</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>0.79213875995945504</v>
+        <v>0.50418966227800732</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>0.58354682017610782</v>
+        <v>0.35789267429157523</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>0.74644057712927547</v>
+        <v>0.45082170644060554</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>0.90082285670725526</v>
+        <v>0.50582692017245301</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>0.97074435782523882</v>
+        <v>0.75990210820240955</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>0.95617913651724429</v>
+        <v>0.93188476858967106</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>0.90519037976198935</v>
+        <v>0.63261795801119336</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>0.98966254826349265</v>
+        <v>0.71603325282104247</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>0.90395332157980868</v>
+        <v>0.41877472951438482</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>0.95101747326323038</v>
+        <v>0.45029451839374096</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>0.86951845002081851</v>
+        <v>0.55159041480602233</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>0.86201622958673951</v>
+        <v>0.21753602570423891</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>0.97852088631629597</v>
+        <v>0.70816525444993794</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>0.90685411478671685</v>
+        <v>0.26607848480272622</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>0.88519322314572502</v>
+        <v>0.46411755984161318</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>0.91020032249677352</v>
+        <v>0.42320062138521458</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>0.84203897793394678</v>
+        <v>0.37204549830118205</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>0.76873185008104206</v>
+        <v>0.38968218796911197</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>0.38957022663427937</v>
+        <v>0.11838791042231629</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>0.65481456252844095</v>
+        <v>0.23460144710516165</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>0.82306485211189484</v>
+        <v>0.34411427128675631</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>0.78356446825979209</v>
+        <v>0.26618944631227137</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>0.93654207494433184</v>
+        <v>0.51063751364053522</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>0.9278027478255525</v>
+        <v>0.7793694420033549</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>0.85232709454638345</v>
+        <v>0.59031136082192182</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>0.76646820383852443</v>
+        <v>0.49195515928793193</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>0.73746866536288791</v>
+        <v>0.40614376085860787</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>0.68073226691763944</v>
+        <v>0.28144891399238653</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>0.68177057156359222</v>
+        <v>0.43634815451011644</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>0.72184603234266653</v>
+        <v>0.4788471911106883</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>0.74083667421926058</v>
+        <v>0.53623690774424926</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>0.75160062579001785</v>
+        <v>0.65717598975673075</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>0.78488690954473994</v>
+        <v>0.63282415393669345</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>0.83819656042400037</v>
+        <v>0.61792245577754978</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>0.89222673861145441</v>
+        <v>0.68390616001298077</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>0.8872478642101963</v>
+        <v>0.75938427746658632</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>0.74988121929694218</v>
+        <v>0.7329978821339167</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>0.67516917310313118</v>
+        <v>0.54448793302708565</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>0.6154415325967828</v>
+        <v>0.62269387219607408</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>0.35744575999975448</v>
+        <v>0.51084871034225199</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>0.80094839628484482</v>
+        <v>0.50755833729248578</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>0.6687280597777715</v>
+        <v>0.50476852743873268</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>0.49660616889882159</v>
+        <v>0.40218982826403404</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>0.50695351869511351</v>
+        <v>0.38992199911065317</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>0.53978684326592752</v>
+        <v>0.5122740680925727</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>0.57405897300873265</v>
+        <v>0.49535974919221276</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>0.43624083667394725</v>
+        <v>0.41574240562373316</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>0.43009958735256826</v>
+        <v>0.44898853295496383</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>0.48737412029001603</v>
+        <v>0.45603919224192818</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0">
-        <v>0.4622928594478844</v>
+        <v>0.55085652015211994</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0">
-        <v>0.50880292901396063</v>
+        <v>0.54411015823651876</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0">
-        <v>0.52153856235791141</v>
+        <v>0.57396182234821236</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0">
-        <v>0.7123852311482286</v>
+        <v>0.6093070899113896</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0">
-        <v>0.51284638106051161</v>
+        <v>0.65280971383297948</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0">
-        <v>0.44962574472099026</v>
+        <v>0.53256440202563649</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0">
-        <v>0.45120582479791438</v>
+        <v>0.49913475680082209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>